<commit_message>
change the create Product log
</commit_message>
<xml_diff>
--- a/Create Product Backlog (Sponsor inputs + Backlog Template).xlsx
+++ b/Create Product Backlog (Sponsor inputs + Backlog Template).xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="51">
   <si>
     <t>#</t>
   </si>
@@ -88,6 +88,15 @@
     <t>as a customer, I want to create an account so that I can sign up in the app</t>
   </si>
   <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
     <t>as a customer, I want to create an account so that I can find all my information and history on the app</t>
   </si>
   <si>
@@ -97,10 +106,25 @@
     <t>as a customer, I want to view restaurants so that I know the details of the restaurant I order from</t>
   </si>
   <si>
+    <t>Open</t>
+  </si>
+  <si>
     <t>as a customer, I want to view restaurants so that I can order based on a specific category of restaurants</t>
   </si>
   <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Todo</t>
+  </si>
+  <si>
     <t>as a customer, I want to view restaurants so that I can find the restaurants near from me</t>
+  </si>
+  <si>
+    <t>Low</t>
   </si>
   <si>
     <t>as a customer, I want to search restaurants so that I find a specific restaurant</t>
@@ -191,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -209,6 +233,9 @@
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2030,10 +2057,18 @@
       <c r="C2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="D2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="3"/>
@@ -2041,12 +2076,20 @@
         <v>2</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="E3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="3"/>
@@ -2054,12 +2097,20 @@
         <v>2</v>
       </c>
       <c r="C4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="F4" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="3"/>
@@ -2074,12 +2125,20 @@
         <v>3</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="3"/>
@@ -2087,12 +2146,20 @@
         <v>3</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="3"/>
@@ -2100,12 +2167,20 @@
         <v>3</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+        <v>34</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="3"/>
@@ -2120,12 +2195,20 @@
         <v>4</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+        <v>36</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="3"/>
@@ -2133,12 +2216,20 @@
         <v>4</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+        <v>37</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="3"/>
@@ -2153,12 +2244,20 @@
         <v>5</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
+        <v>38</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="3"/>
@@ -2166,12 +2265,20 @@
         <v>5</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
+        <v>39</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="3"/>
@@ -2193,12 +2300,20 @@
         <v>6</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
+        <v>40</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="3"/>
@@ -2206,12 +2321,20 @@
         <v>6</v>
       </c>
       <c r="C18" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="G18" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="3"/>
@@ -2219,12 +2342,20 @@
         <v>6</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
+        <v>42</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="3"/>
@@ -2232,12 +2363,20 @@
         <v>6</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
+        <v>43</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="3"/>
@@ -2259,12 +2398,20 @@
         <v>7</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
+        <v>44</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="3"/>
@@ -2272,12 +2419,20 @@
         <v>7</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
+        <v>45</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="3"/>
@@ -2285,12 +2440,20 @@
         <v>7</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
+        <v>46</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="3"/>
@@ -2305,12 +2468,20 @@
         <v>8</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
+        <v>47</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="3"/>
@@ -2318,12 +2489,20 @@
         <v>8</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
+        <v>48</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F28" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="3"/>
@@ -2339,12 +2518,20 @@
         <v>9</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
+        <v>49</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="3"/>
@@ -2352,12 +2539,20 @@
         <v>9</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
+        <v>50</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F31" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="3"/>

</xml_diff>